<commit_message>
Updated Capital_Goods.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Capital_Goods.xlsx
+++ b/NAV/Capital_Goods.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J612"/>
+  <dimension ref="A1:J633"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A577" workbookViewId="0">
       <selection activeCell="E605" sqref="E605"/>
@@ -19491,6 +19491,657 @@
         <v>338.796762044303</v>
       </c>
     </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>2024-08-28</t>
+        </is>
+      </c>
+      <c r="C613" t="n">
+        <v>1890.599975585938</v>
+      </c>
+      <c r="D613" t="n">
+        <v>711.7999877929688</v>
+      </c>
+      <c r="E613" t="n">
+        <v>78.95999908447266</v>
+      </c>
+      <c r="F613" t="n">
+        <v>299.9500122070312</v>
+      </c>
+      <c r="G613" t="n">
+        <v>1323.25</v>
+      </c>
+      <c r="H613" t="n">
+        <v>29275.72984313965</v>
+      </c>
+      <c r="I613" t="n">
+        <v>0</v>
+      </c>
+      <c r="J613" t="n">
+        <v>338.796762044303</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="C614" t="n">
+        <v>1893.25</v>
+      </c>
+      <c r="D614" t="n">
+        <v>700.7999877929688</v>
+      </c>
+      <c r="E614" t="n">
+        <v>77</v>
+      </c>
+      <c r="F614" t="n">
+        <v>296.2000122070312</v>
+      </c>
+      <c r="G614" t="n">
+        <v>1298.650024414062</v>
+      </c>
+      <c r="H614" t="n">
+        <v>28928.15008544922</v>
+      </c>
+      <c r="I614" t="n">
+        <v>-0.01187262485180639</v>
+      </c>
+      <c r="J614" t="n">
+        <v>334.7743551875443</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C615" t="n">
+        <v>1899.349975585938</v>
+      </c>
+      <c r="D615" t="n">
+        <v>696.0999755859375</v>
+      </c>
+      <c r="E615" t="n">
+        <v>75.83999633789062</v>
+      </c>
+      <c r="F615" t="n">
+        <v>299.2999877929688</v>
+      </c>
+      <c r="G615" t="n">
+        <v>1302.900024414062</v>
+      </c>
+      <c r="H615" t="n">
+        <v>28869.96923828125</v>
+      </c>
+      <c r="I615" t="n">
+        <v>-0.002011219071945895</v>
+      </c>
+      <c r="J615" t="n">
+        <v>334.1010506195927</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>1885.400024414062</v>
+      </c>
+      <c r="D616" t="n">
+        <v>683.5999755859375</v>
+      </c>
+      <c r="E616" t="n">
+        <v>73.80999755859375</v>
+      </c>
+      <c r="F616" t="n">
+        <v>296.8999938964844</v>
+      </c>
+      <c r="G616" t="n">
+        <v>1303.849975585938</v>
+      </c>
+      <c r="H616" t="n">
+        <v>28487.57955932617</v>
+      </c>
+      <c r="I616" t="n">
+        <v>-0.01324524026329871</v>
+      </c>
+      <c r="J616" t="n">
+        <v>329.6758019319157</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C617" t="n">
+        <v>1901.949951171875</v>
+      </c>
+      <c r="D617" t="n">
+        <v>689.4000244140625</v>
+      </c>
+      <c r="E617" t="n">
+        <v>74.47000122070312</v>
+      </c>
+      <c r="F617" t="n">
+        <v>297.1499938964844</v>
+      </c>
+      <c r="G617" t="n">
+        <v>1320.25</v>
+      </c>
+      <c r="H617" t="n">
+        <v>28715.86001586914</v>
+      </c>
+      <c r="I617" t="n">
+        <v>0.008013332830455756</v>
+      </c>
+      <c r="J617" t="n">
+        <v>332.3176038589435</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C618" t="n">
+        <v>1901.300048828125</v>
+      </c>
+      <c r="D618" t="n">
+        <v>688.9500122070312</v>
+      </c>
+      <c r="E618" t="n">
+        <v>74.16000366210938</v>
+      </c>
+      <c r="F618" t="n">
+        <v>298.9500122070312</v>
+      </c>
+      <c r="G618" t="n">
+        <v>1327.099975585938</v>
+      </c>
+      <c r="H618" t="n">
+        <v>28721.03076171875</v>
+      </c>
+      <c r="I618" t="n">
+        <v>0.0001800658537390795</v>
+      </c>
+      <c r="J618" t="n">
+        <v>332.3774429119949</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C619" t="n">
+        <v>1879.449951171875</v>
+      </c>
+      <c r="D619" t="n">
+        <v>687.5</v>
+      </c>
+      <c r="E619" t="n">
+        <v>76</v>
+      </c>
+      <c r="F619" t="n">
+        <v>290.6000061035156</v>
+      </c>
+      <c r="G619" t="n">
+        <v>1312.349975585938</v>
+      </c>
+      <c r="H619" t="n">
+        <v>28602.74978637695</v>
+      </c>
+      <c r="I619" t="n">
+        <v>-0.004118270556621158</v>
+      </c>
+      <c r="J619" t="n">
+        <v>331.0086226751654</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C620" t="n">
+        <v>1872.349975585938</v>
+      </c>
+      <c r="D620" t="n">
+        <v>673.5499877929688</v>
+      </c>
+      <c r="E620" t="n">
+        <v>74.72000122070312</v>
+      </c>
+      <c r="F620" t="n">
+        <v>283.6000061035156</v>
+      </c>
+      <c r="G620" t="n">
+        <v>1289.699951171875</v>
+      </c>
+      <c r="H620" t="n">
+        <v>28191.60983276367</v>
+      </c>
+      <c r="I620" t="n">
+        <v>-0.01437414083205038</v>
+      </c>
+      <c r="J620" t="n">
+        <v>326.2506581162095</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C621" t="n">
+        <v>1892.400024414062</v>
+      </c>
+      <c r="D621" t="n">
+        <v>664.1500244140625</v>
+      </c>
+      <c r="E621" t="n">
+        <v>74.33999633789062</v>
+      </c>
+      <c r="F621" t="n">
+        <v>281.5499877929688</v>
+      </c>
+      <c r="G621" t="n">
+        <v>1237.150024414062</v>
+      </c>
+      <c r="H621" t="n">
+        <v>28036.46997070312</v>
+      </c>
+      <c r="I621" t="n">
+        <v>-0.005503050836077006</v>
+      </c>
+      <c r="J621" t="n">
+        <v>324.4552841592924</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C622" t="n">
+        <v>1922.449951171875</v>
+      </c>
+      <c r="D622" t="n">
+        <v>664.5999755859375</v>
+      </c>
+      <c r="E622" t="n">
+        <v>78.05000305175781</v>
+      </c>
+      <c r="F622" t="n">
+        <v>285.75</v>
+      </c>
+      <c r="G622" t="n">
+        <v>1250.300048828125</v>
+      </c>
+      <c r="H622" t="n">
+        <v>28561.49984741211</v>
+      </c>
+      <c r="I622" t="n">
+        <v>0.01872667555001102</v>
+      </c>
+      <c r="J622" t="n">
+        <v>330.5312529962301</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C623" t="n">
+        <v>1957.599975585938</v>
+      </c>
+      <c r="D623" t="n">
+        <v>689.75</v>
+      </c>
+      <c r="E623" t="n">
+        <v>81.94999694824219</v>
+      </c>
+      <c r="F623" t="n">
+        <v>288.0499877929688</v>
+      </c>
+      <c r="G623" t="n">
+        <v>1237.699951171875</v>
+      </c>
+      <c r="H623" t="n">
+        <v>29297.64938354492</v>
+      </c>
+      <c r="I623" t="n">
+        <v>0.0257741904334731</v>
+      </c>
+      <c r="J623" t="n">
+        <v>339.0504284551695</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C624" t="n">
+        <v>1996.400024414062</v>
+      </c>
+      <c r="D624" t="n">
+        <v>729.1500244140625</v>
+      </c>
+      <c r="E624" t="n">
+        <v>81.69999694824219</v>
+      </c>
+      <c r="F624" t="n">
+        <v>291.7000122070312</v>
+      </c>
+      <c r="G624" t="n">
+        <v>1237.300048828125</v>
+      </c>
+      <c r="H624" t="n">
+        <v>29912.80038452148</v>
+      </c>
+      <c r="I624" t="n">
+        <v>0.02099659917843318</v>
+      </c>
+      <c r="J624" t="n">
+        <v>346.1693344027187</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C625" t="n">
+        <v>1988.050048828125</v>
+      </c>
+      <c r="D625" t="n">
+        <v>713.7000122070312</v>
+      </c>
+      <c r="E625" t="n">
+        <v>83.11000061035156</v>
+      </c>
+      <c r="F625" t="n">
+        <v>289.9500122070312</v>
+      </c>
+      <c r="G625" t="n">
+        <v>1241.5</v>
+      </c>
+      <c r="H625" t="n">
+        <v>29812.18057250977</v>
+      </c>
+      <c r="I625" t="n">
+        <v>-0.003363771051799782</v>
+      </c>
+      <c r="J625" t="n">
+        <v>345.004900016634</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C626" t="n">
+        <v>1989.900024414062</v>
+      </c>
+      <c r="D626" t="n">
+        <v>714.2000122070312</v>
+      </c>
+      <c r="E626" t="n">
+        <v>84.69999694824219</v>
+      </c>
+      <c r="F626" t="n">
+        <v>290.3999938964844</v>
+      </c>
+      <c r="G626" t="n">
+        <v>1226.599975585938</v>
+      </c>
+      <c r="H626" t="n">
+        <v>29926.49987792969</v>
+      </c>
+      <c r="I626" t="n">
+        <v>0.003834650911961043</v>
+      </c>
+      <c r="J626" t="n">
+        <v>346.3278733711138</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C627" t="n">
+        <v>2006.550048828125</v>
+      </c>
+      <c r="D627" t="n">
+        <v>731.0999755859375</v>
+      </c>
+      <c r="E627" t="n">
+        <v>82</v>
+      </c>
+      <c r="F627" t="n">
+        <v>284.2999877929688</v>
+      </c>
+      <c r="G627" t="n">
+        <v>1193.800048828125</v>
+      </c>
+      <c r="H627" t="n">
+        <v>29823.24993896484</v>
+      </c>
+      <c r="I627" t="n">
+        <v>-0.003450117433913109</v>
+      </c>
+      <c r="J627" t="n">
+        <v>345.1330015373461</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C628" t="n">
+        <v>1987.800048828125</v>
+      </c>
+      <c r="D628" t="n">
+        <v>743.25</v>
+      </c>
+      <c r="E628" t="n">
+        <v>80.81999969482422</v>
+      </c>
+      <c r="F628" t="n">
+        <v>282.8500061035156</v>
+      </c>
+      <c r="G628" t="n">
+        <v>1166.400024414062</v>
+      </c>
+      <c r="H628" t="n">
+        <v>29685.31034851074</v>
+      </c>
+      <c r="I628" t="n">
+        <v>-0.004625236710834788</v>
+      </c>
+      <c r="J628" t="n">
+        <v>343.536679708515</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C629" t="n">
+        <v>1998.599975585938</v>
+      </c>
+      <c r="D629" t="n">
+        <v>735.9500122070312</v>
+      </c>
+      <c r="E629" t="n">
+        <v>80.97000122070312</v>
+      </c>
+      <c r="F629" t="n">
+        <v>272.7000122070312</v>
+      </c>
+      <c r="G629" t="n">
+        <v>1121.300048828125</v>
+      </c>
+      <c r="H629" t="n">
+        <v>29455.8603515625</v>
+      </c>
+      <c r="I629" t="n">
+        <v>-0.0077294120982553</v>
+      </c>
+      <c r="J629" t="n">
+        <v>340.8813431401815</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C630" t="n">
+        <v>2048.10009765625</v>
+      </c>
+      <c r="D630" t="n">
+        <v>746.5</v>
+      </c>
+      <c r="E630" t="n">
+        <v>83.44999694824219</v>
+      </c>
+      <c r="F630" t="n">
+        <v>277.3500061035156</v>
+      </c>
+      <c r="G630" t="n">
+        <v>1149.400024414062</v>
+      </c>
+      <c r="H630" t="n">
+        <v>30118.95037841797</v>
+      </c>
+      <c r="I630" t="n">
+        <v>0.02251131078642199</v>
+      </c>
+      <c r="J630" t="n">
+        <v>348.5550289969032</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>2082.39990234375</v>
+      </c>
+      <c r="D631" t="n">
+        <v>773.9500122070312</v>
+      </c>
+      <c r="E631" t="n">
+        <v>82.88999938964844</v>
+      </c>
+      <c r="F631" t="n">
+        <v>286.2999877929688</v>
+      </c>
+      <c r="G631" t="n">
+        <v>1162.75</v>
+      </c>
+      <c r="H631" t="n">
+        <v>30664.31942749023</v>
+      </c>
+      <c r="I631" t="n">
+        <v>0.01810717313253569</v>
+      </c>
+      <c r="J631" t="n">
+        <v>354.8663752531661</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="C632" t="n">
+        <v>2068.14990234375</v>
+      </c>
+      <c r="D632" t="n">
+        <v>781.8499755859375</v>
+      </c>
+      <c r="E632" t="n">
+        <v>83.79000091552734</v>
+      </c>
+      <c r="F632" t="n">
+        <v>291.7999877929688</v>
+      </c>
+      <c r="G632" t="n">
+        <v>1141.199951171875</v>
+      </c>
+      <c r="H632" t="n">
+        <v>30770.6690826416</v>
+      </c>
+      <c r="I632" t="n">
+        <v>0.003468188994144963</v>
+      </c>
+      <c r="J632" t="n">
+        <v>356.0971189102113</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="C633" t="n">
+        <v>2061.60009765625</v>
+      </c>
+      <c r="D633" t="n">
+        <v>775.8499755859375</v>
+      </c>
+      <c r="E633" t="n">
+        <v>82.95999908447266</v>
+      </c>
+      <c r="F633" t="n">
+        <v>289.8500061035156</v>
+      </c>
+      <c r="G633" t="n">
+        <v>1118.449951171875</v>
+      </c>
+      <c r="H633" t="n">
+        <v>30542.33015441895</v>
+      </c>
+      <c r="I633" t="n">
+        <v>-0.007420668286718119</v>
+      </c>
+      <c r="J633" t="n">
+        <v>353.4546403129226</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>